<commit_message>
Iniciando limpeza de tweets
</commit_message>
<xml_diff>
--- a/mandalorian.xlsx
+++ b/mandalorian.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Documents\INSPER\2_Semestre\C_Dados\Projeto 1\TheMandalorian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1dd2b3b0fc327b09/Documentos/Arquivos INSPER 2° SEMESTRE/C-Dados/TheMandalorian/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ED08CF-40A2-472C-90C4-D98FB2F34A21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{70ED08CF-40A2-472C-90C4-D98FB2F34A21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC33C3CC-85A3-4D32-AE02-66CFCDF89EF3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1610" yWindow="1400" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2672,12 +2672,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3016,10 +3019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B501"/>
+  <dimension ref="A1:D501"/>
   <sheetViews>
-    <sheetView topLeftCell="A450" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B501" sqref="B501"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3028,7 +3031,7 @@
     <col min="2" max="2" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3036,15 +3039,15 @@
         <v>726</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3052,7 +3055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3068,15 +3071,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3084,7 +3088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3092,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3100,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3108,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3116,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3124,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3132,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3140,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3148,7 +3152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -3476,8 +3480,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="57" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B57">
@@ -7046,8 +7050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D230" sqref="D230"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>